<commit_message>
11.1 Identificación de bases de datos
</commit_message>
<xml_diff>
--- a/estadoDelArte/mapasMentales/deteccionActividades/AnalisisDeteccionActividades_completo.xlsx
+++ b/estadoDelArte/mapasMentales/deteccionActividades/AnalisisDeteccionActividades_completo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Personal Projects\dauruxu\estadoDelArte\mapasMentales\deteccionActividades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\dauruxu\estadoDelArte\mapasMentales\deteccionActividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6B77C-DA77-4EC4-A8D7-8DE6DC4DCFA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB992C7-DE31-4E94-9E5A-0B6C348DB29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revisión" sheetId="2" r:id="rId1"/>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>clasificación de acciones en curso, desarrollados en base a clasificadores y modelos temporales de última generación: SVM ( Vapnik, 1998 ), HMM ( Rabiner, 1989 ) y LSTM ( Hochreiter y Schmidhuber, 1997 ). Estos métodos tienen diferentes filosofías de reconocimiento . La evaluación de todos los métodos se lleva a cabo utilizando datos idénticos.</t>
-  </si>
-  <si>
-    <t>Conjunto de datos Montalbano Gesture ( Escalera et al., 2014 ), el conjunto de datos MPII Cooking 2 ( Rohrbach et al., 2015 ) y el conjunto de datos ActivityNet ( Fabian Caba Heilbron et al., 2015 ).</t>
   </si>
   <si>
     <t>Ekta Vats, Chee Seng Chan∗</t>
@@ -362,6 +359,9 @@
   </si>
   <si>
     <t>70%-88%</t>
+  </si>
+  <si>
+    <t>Conjunto de datos Montalbano Gesture ( Escalera et al., 2014 ), el conjunto de datos MPII Cooking 2 ( Rohrbach et al., 2015 ) y el conjunto de datos ActivityNet ( Fabian Caba Heilbron et al., 2015 ).http://chalearnlap.cvc.uab.es/dataset/21/associated-events/</t>
   </si>
 </sst>
 </file>
@@ -1908,8 +1908,8 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1927,7 +1927,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1948,7 +1948,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>6</v>
@@ -1959,10 +1959,10 @@
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="190.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
@@ -1980,7 +1980,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="201.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -2010,14 +2010,14 @@
         <v>17</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" s="5" customFormat="1" ht="187.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>19</v>
@@ -2029,16 +2029,16 @@
         <v>2018</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>21</v>
@@ -2047,207 +2047,207 @@
     </row>
     <row r="5" spans="1:10" s="5" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="9">
         <v>2016</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" s="5" customFormat="1" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="9">
         <v>2017</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="H6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" s="5" customFormat="1" ht="330.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D7" s="9">
         <v>2014</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1" ht="304.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="10">
         <v>2018</v>
       </c>
       <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" s="5" customFormat="1" ht="345.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="10">
         <v>2013</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="259.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="D10" s="10">
         <v>2017</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="369.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="D11" s="10">
         <v>2004</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="G11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="7"/>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D69" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>